<commit_message>
probando guardar automatico en pc maribel tienda
</commit_message>
<xml_diff>
--- a/INVENTARIOS DEPOSITO/14-07-2022/david 17-7-2022 BOTIN AIR FORCE.xlsx
+++ b/INVENTARIOS DEPOSITO/14-07-2022/david 17-7-2022 BOTIN AIR FORCE.xlsx
@@ -5,27 +5,58 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABDALLA\Desktop\INVENTARIOS\INVENTARIOS DEPOSITO\14-07-2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b11507c57360364/Escritorio/INVENTARIOS/INVENTARIOS DEPOSITO/14-07-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33F1AA1-4773-47F1-99C9-306CE874764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D33F1AA1-4773-47F1-99C9-306CE874764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE682B47-45DF-4511-8BDC-BFD2C131AF11}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBD3A55A-80AB-4B27-8CE0-5C4B9B08D856}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="50">
   <si>
     <t>CO_ART</t>
   </si>
@@ -144,47 +175,44 @@
     <t>0005700003577CI11</t>
   </si>
   <si>
-    <t>NBA41LAK-20002</t>
-  </si>
-  <si>
-    <t>NBA40LAK-20002</t>
-  </si>
-  <si>
-    <t>NBA43LAK-20002</t>
-  </si>
-  <si>
-    <t>NBA44LAK-20002</t>
-  </si>
-  <si>
     <t>BOTIN NIKE AIR FORCE LAKERS BLANCO AMARILLO MORADO</t>
   </si>
   <si>
     <t>BLANCO AMARRILLO</t>
   </si>
   <si>
-    <t>NBC40ARC-30003</t>
-  </si>
-  <si>
     <t>BOTIN NIKER AIR FORCE BLANCO ARCOIRIS AZUL AMARRILO</t>
   </si>
   <si>
-    <t>NBC41ARC-30003</t>
-  </si>
-  <si>
-    <t>NBC42ARC-30003</t>
-  </si>
-  <si>
-    <t>NBC43ARC-30003</t>
-  </si>
-  <si>
-    <t>NBC44ARC-30003</t>
+    <t>NBA41LAK-10001</t>
+  </si>
+  <si>
+    <t>NBA43LAK-10001</t>
+  </si>
+  <si>
+    <t>NBA44LAK-10001</t>
+  </si>
+  <si>
+    <t>NBC40ARC-10001</t>
+  </si>
+  <si>
+    <t>NBC41ARC-10001</t>
+  </si>
+  <si>
+    <t>NBC42ARC-10001</t>
+  </si>
+  <si>
+    <t>NBC43ARC-10001</t>
+  </si>
+  <si>
+    <t>NBC44ARC-10001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +223,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -563,15 +597,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EB4220-DEDD-4608-B2E0-D0A1E0FC381A}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="53.140625" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.7109375" customWidth="1"/>
@@ -810,7 +844,7 @@
         <v>37</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4">
         <v>1</v>
@@ -869,7 +903,7 @@
         <v>37</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <v>1</v>
@@ -895,10 +929,10 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -919,10 +953,10 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J6">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K6" t="s">
         <v>37</v>
@@ -948,16 +982,17 @@
       <c r="Y6">
         <v>5</v>
       </c>
-      <c r="Z6" t="s">
-        <v>35</v>
+      <c r="Z6" t="e" cm="1">
+        <f t="array" ref="Z6">#REF!:Z11AIR FORCE</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
@@ -978,16 +1013,16 @@
         <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
         <v>37</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <v>1</v>
@@ -1013,10 +1048,10 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1037,10 +1072,10 @@
         <v>35</v>
       </c>
       <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8">
         <v>44</v>
-      </c>
-      <c r="J8">
-        <v>43</v>
       </c>
       <c r="K8" t="s">
         <v>37</v>
@@ -1072,10 +1107,10 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -1096,10 +1131,10 @@
         <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J9">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
         <v>37</v>
@@ -1131,10 +1166,10 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1155,10 +1190,10 @@
         <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J10">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K10" t="s">
         <v>37</v>
@@ -1193,7 +1228,7 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1214,10 +1249,10 @@
         <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J11">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K11" t="s">
         <v>37</v>
@@ -1252,7 +1287,7 @@
         <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -1273,16 +1308,16 @@
         <v>35</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J12">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
         <v>37</v>
       </c>
       <c r="N12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T12">
         <v>1</v>
@@ -1311,7 +1346,7 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1332,10 +1367,10 @@
         <v>35</v>
       </c>
       <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13">
         <v>44</v>
-      </c>
-      <c r="J13">
-        <v>43</v>
       </c>
       <c r="K13" t="s">
         <v>37</v>
@@ -1365,45 +1400,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14">
-        <v>44</v>
-      </c>
-      <c r="K14" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>